<commit_message>
menambahkan fungsi spinner saat unggah file besar
</commit_message>
<xml_diff>
--- a/data/data_aging_multi_column.xlsx
+++ b/data/data_aging_multi_column.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\magang\python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\magang\python\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44440988-A698-4458-8E70-0349DC38B0B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6938F52-FCAE-430D-A77A-6F49E51A7954}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -471,7 +471,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,7 +645,10 @@
         <v>25</v>
       </c>
       <c r="C11">
-        <v>12392968</v>
+        <v>596141</v>
+      </c>
+      <c r="E11">
+        <v>596141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>